<commit_message>
Cleaned up the data files a little bit.
</commit_message>
<xml_diff>
--- a/Colour Measurements.xlsx
+++ b/Colour Measurements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessiepan/Desktop/Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Dropbox (Personal)\Jessie Pan\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CADFF35-0096-B54A-B884-8E6C06BB1761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4436F5B2-CABF-4666-936D-0591087C1388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2CA9E0D8-87C5-8D45-9A41-680465435F7B}"/>
+    <workbookView xWindow="2674" yWindow="1406" windowWidth="28817" windowHeight="15325" xr2:uid="{2CA9E0D8-87C5-8D45-9A41-680465435F7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="73">
   <si>
     <t>Tree Name</t>
   </si>
@@ -254,40 +254,13 @@
   </si>
   <si>
     <t>#9A784E</t>
-  </si>
-  <si>
-    <t>Total Transmittance</t>
-  </si>
-  <si>
-    <t>Specular Transmittance</t>
-  </si>
-  <si>
-    <t>Diffuse Transmittance</t>
-  </si>
-  <si>
-    <t>Object Type</t>
-  </si>
-  <si>
-    <t>OpaqueORTransparent</t>
-  </si>
-  <si>
-    <t>Radiance Type</t>
-  </si>
-  <si>
-    <t>Plant</t>
-  </si>
-  <si>
-    <t>Opaque</t>
-  </si>
-  <si>
-    <t>Plastic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -326,14 +299,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="49">
     <fill>
@@ -637,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -690,7 +655,6 @@
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1019,15 +983,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{930148F6-2425-1840-9670-DC77496BEFA6}">
-  <dimension ref="A2:U74"/>
+  <dimension ref="A2:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="67" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="67" workbookViewId="0">
+      <selection activeCell="U64" sqref="U64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1052,35 +1016,17 @@
       <c r="K2" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="L2" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="M2" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="S2" s="52" t="s">
-        <v>73</v>
-      </c>
-      <c r="T2" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="U2" s="52" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1095,20 +1041,13 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -1137,35 +1076,17 @@
       <c r="K5">
         <v>18.75</v>
       </c>
+      <c r="L5">
+        <v>2.0000000000000001E-4</v>
+      </c>
       <c r="M5">
-        <v>2.0000000000000001E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="P5" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>80</v>
-      </c>
-      <c r="R5" t="s">
-        <v>81</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
         <v>17</v>
@@ -1192,35 +1113,17 @@
       <c r="K6">
         <v>8.81</v>
       </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
       <c r="M6">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
         <v>0.28050000000000003</v>
       </c>
-      <c r="P6" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>80</v>
-      </c>
-      <c r="R6" t="s">
-        <v>81</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -1249,35 +1152,17 @@
       <c r="K7">
         <v>13.03</v>
       </c>
+      <c r="L7">
+        <v>6.9999999999999999E-4</v>
+      </c>
       <c r="M7">
-        <v>6.9999999999999999E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
         <v>8.6199999999999999E-2</v>
       </c>
-      <c r="P7" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>80</v>
-      </c>
-      <c r="R7" t="s">
-        <v>81</v>
-      </c>
-      <c r="S7">
-        <v>0</v>
-      </c>
-      <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
         <v>17</v>
@@ -1304,43 +1189,25 @@
       <c r="K8">
         <v>4.53</v>
       </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
       <c r="M8">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
         <v>0.25879999999999997</v>
       </c>
-      <c r="P8" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>80</v>
-      </c>
-      <c r="R8" t="s">
-        <v>81</v>
-      </c>
-      <c r="S8">
-        <v>0</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1369,35 +1236,17 @@
       <c r="K11">
         <v>16.510000000000002</v>
       </c>
+      <c r="L11">
+        <v>2.0000000000000001E-4</v>
+      </c>
       <c r="M11">
-        <v>2.0000000000000001E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="P11" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>80</v>
-      </c>
-      <c r="R11" t="s">
-        <v>81</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>17</v>
@@ -1424,35 +1273,17 @@
       <c r="K12">
         <v>21.64</v>
       </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
       <c r="M12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12">
         <v>0.17449999999999999</v>
       </c>
-      <c r="P12" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>80</v>
-      </c>
-      <c r="R12" t="s">
-        <v>81</v>
-      </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1460,21 +1291,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -1503,35 +1334,17 @@
       <c r="K17">
         <v>7.98</v>
       </c>
+      <c r="L17">
+        <v>2.2000000000000001E-3</v>
+      </c>
       <c r="M17">
-        <v>2.2000000000000001E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="P17" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>80</v>
-      </c>
-      <c r="R17" t="s">
-        <v>81</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-      <c r="T17">
-        <v>0</v>
-      </c>
-      <c r="U17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>17</v>
@@ -1558,35 +1371,17 @@
       <c r="K18">
         <v>17.57</v>
       </c>
+      <c r="L18">
+        <v>1.6000000000000001E-3</v>
+      </c>
       <c r="M18">
-        <v>1.6000000000000001E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
         <v>0.16289999999999999</v>
       </c>
-      <c r="P18" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>80</v>
-      </c>
-      <c r="R18" t="s">
-        <v>81</v>
-      </c>
-      <c r="S18">
-        <v>0</v>
-      </c>
-      <c r="T18">
-        <v>0</v>
-      </c>
-      <c r="U18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -1615,35 +1410,17 @@
       <c r="K19">
         <v>48.89</v>
       </c>
+      <c r="L19">
+        <v>3.3999999999999998E-3</v>
+      </c>
       <c r="M19">
-        <v>3.3999999999999998E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
         <v>0.38300000000000001</v>
       </c>
-      <c r="P19" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>80</v>
-      </c>
-      <c r="R19" t="s">
-        <v>81</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-      <c r="T19">
-        <v>0</v>
-      </c>
-      <c r="U19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" s="5"/>
       <c r="B20" s="5" t="s">
         <v>17</v>
@@ -1670,40 +1447,22 @@
       <c r="K20">
         <v>32.42</v>
       </c>
+      <c r="L20">
+        <v>3.0000000000000001E-3</v>
+      </c>
       <c r="M20">
-        <v>3.0000000000000001E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
         <v>0.38379999999999997</v>
       </c>
-      <c r="P20" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>80</v>
-      </c>
-      <c r="R20" t="s">
-        <v>81</v>
-      </c>
-      <c r="S20">
-        <v>0</v>
-      </c>
-      <c r="T20">
-        <v>0</v>
-      </c>
-      <c r="U20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>15</v>
       </c>
@@ -1732,35 +1491,17 @@
       <c r="K23">
         <v>11.89</v>
       </c>
+      <c r="L23">
+        <v>2.0000000000000001E-4</v>
+      </c>
       <c r="M23">
-        <v>2.0000000000000001E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
         <v>8.4099999999999994E-2</v>
       </c>
-      <c r="P23" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>80</v>
-      </c>
-      <c r="R23" t="s">
-        <v>81</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-      <c r="T23">
-        <v>0</v>
-      </c>
-      <c r="U23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A24" s="5"/>
       <c r="B24" s="5" t="s">
         <v>17</v>
@@ -1787,35 +1528,17 @@
       <c r="K24">
         <v>22.4</v>
       </c>
+      <c r="L24">
+        <v>2.9999999999999997E-4</v>
+      </c>
       <c r="M24">
-        <v>2.9999999999999997E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
         <v>0.1547</v>
       </c>
-      <c r="P24" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>80</v>
-      </c>
-      <c r="R24" t="s">
-        <v>81</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-      <c r="T24">
-        <v>0</v>
-      </c>
-      <c r="U24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
         <v>18</v>
       </c>
@@ -1844,35 +1567,17 @@
       <c r="K25">
         <v>15.1</v>
       </c>
+      <c r="L25">
+        <v>2.9999999999999997E-4</v>
+      </c>
       <c r="M25">
-        <v>2.9999999999999997E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
         <v>9.2399999999999996E-2</v>
       </c>
-      <c r="P25" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>80</v>
-      </c>
-      <c r="R25" t="s">
-        <v>81</v>
-      </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
-      <c r="T25">
-        <v>0</v>
-      </c>
-      <c r="U25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A26" s="5"/>
       <c r="B26" s="5" t="s">
         <v>17</v>
@@ -1899,40 +1604,22 @@
       <c r="K26">
         <v>21.11</v>
       </c>
+      <c r="L26">
+        <v>4.0000000000000002E-4</v>
+      </c>
       <c r="M26">
-        <v>4.0000000000000002E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
         <v>0.14199999999999999</v>
       </c>
-      <c r="P26" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>80</v>
-      </c>
-      <c r="R26" t="s">
-        <v>81</v>
-      </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <v>0</v>
-      </c>
-      <c r="U26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>15</v>
       </c>
@@ -1961,35 +1648,17 @@
       <c r="K29">
         <v>14.46</v>
       </c>
+      <c r="L29">
+        <v>8.9999999999999998E-4</v>
+      </c>
       <c r="M29">
-        <v>8.9999999999999998E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
         <v>8.6400000000000005E-2</v>
       </c>
-      <c r="P29" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>80</v>
-      </c>
-      <c r="R29" t="s">
-        <v>81</v>
-      </c>
-      <c r="S29">
-        <v>0</v>
-      </c>
-      <c r="T29">
-        <v>0</v>
-      </c>
-      <c r="U29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A30" s="5"/>
       <c r="B30" s="5" t="s">
         <v>17</v>
@@ -2016,35 +1685,17 @@
       <c r="K30">
         <v>24.32</v>
       </c>
+      <c r="L30">
+        <v>1.6999999999999999E-3</v>
+      </c>
       <c r="M30">
-        <v>1.6999999999999999E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N30">
-        <v>0</v>
-      </c>
-      <c r="O30">
         <v>0.19800000000000001</v>
       </c>
-      <c r="P30" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>80</v>
-      </c>
-      <c r="R30" t="s">
-        <v>81</v>
-      </c>
-      <c r="S30">
-        <v>0</v>
-      </c>
-      <c r="T30">
-        <v>0</v>
-      </c>
-      <c r="U30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>18</v>
       </c>
@@ -2073,35 +1724,17 @@
       <c r="K31">
         <v>39.56</v>
       </c>
+      <c r="L31">
+        <v>0</v>
+      </c>
       <c r="M31">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
         <v>0.20219999999999999</v>
       </c>
-      <c r="P31" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>80</v>
-      </c>
-      <c r="R31" t="s">
-        <v>81</v>
-      </c>
-      <c r="S31">
-        <v>0</v>
-      </c>
-      <c r="T31">
-        <v>0</v>
-      </c>
-      <c r="U31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
         <v>17</v>
@@ -2128,43 +1761,25 @@
       <c r="K32">
         <v>36.49</v>
       </c>
+      <c r="L32">
+        <v>2E-3</v>
+      </c>
       <c r="M32">
-        <v>2E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N32">
-        <v>0</v>
-      </c>
-      <c r="O32">
         <v>0.2525</v>
       </c>
-      <c r="P32" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>80</v>
-      </c>
-      <c r="R32" t="s">
-        <v>81</v>
-      </c>
-      <c r="S32">
-        <v>0</v>
-      </c>
-      <c r="T32">
-        <v>0</v>
-      </c>
-      <c r="U32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A35" s="5" t="s">
         <v>15</v>
       </c>
@@ -2193,35 +1808,17 @@
       <c r="K35">
         <v>24.81</v>
       </c>
+      <c r="L35">
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="M35">
-        <v>5.0000000000000001E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35">
         <v>0.1215</v>
       </c>
-      <c r="P35" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>80</v>
-      </c>
-      <c r="R35" t="s">
-        <v>81</v>
-      </c>
-      <c r="S35">
-        <v>0</v>
-      </c>
-      <c r="T35">
-        <v>0</v>
-      </c>
-      <c r="U35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
         <v>17</v>
@@ -2248,35 +1845,17 @@
       <c r="K36">
         <v>19.59</v>
       </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
       <c r="M36">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="N36">
-        <v>0</v>
-      </c>
-      <c r="O36">
         <v>0.2419</v>
       </c>
-      <c r="P36" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q36" t="s">
-        <v>80</v>
-      </c>
-      <c r="R36" t="s">
-        <v>81</v>
-      </c>
-      <c r="S36">
-        <v>0</v>
-      </c>
-      <c r="T36">
-        <v>0</v>
-      </c>
-      <c r="U36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A37" s="5" t="s">
         <v>18</v>
       </c>
@@ -2305,35 +1884,17 @@
       <c r="K37">
         <v>33.85</v>
       </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
       <c r="M37">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="N37">
-        <v>0</v>
-      </c>
-      <c r="O37">
         <v>0.17530000000000001</v>
       </c>
-      <c r="P37" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q37" t="s">
-        <v>80</v>
-      </c>
-      <c r="R37" t="s">
-        <v>81</v>
-      </c>
-      <c r="S37">
-        <v>0</v>
-      </c>
-      <c r="T37">
-        <v>0</v>
-      </c>
-      <c r="U37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A38" s="5"/>
       <c r="B38" s="5" t="s">
         <v>17</v>
@@ -2360,40 +1921,22 @@
       <c r="K38">
         <v>26.58</v>
       </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
       <c r="M38">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="N38">
-        <v>0</v>
-      </c>
-      <c r="O38">
         <v>0.2094</v>
       </c>
-      <c r="P38" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>80</v>
-      </c>
-      <c r="R38" t="s">
-        <v>81</v>
-      </c>
-      <c r="S38">
-        <v>0</v>
-      </c>
-      <c r="T38">
-        <v>0</v>
-      </c>
-      <c r="U38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A41" s="5" t="s">
         <v>15</v>
       </c>
@@ -2422,35 +1965,17 @@
       <c r="K41">
         <v>16.73</v>
       </c>
+      <c r="L41">
+        <v>2.9999999999999997E-4</v>
+      </c>
       <c r="M41">
-        <v>2.9999999999999997E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N41">
-        <v>0</v>
-      </c>
-      <c r="O41">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="P41" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q41" t="s">
-        <v>80</v>
-      </c>
-      <c r="R41" t="s">
-        <v>81</v>
-      </c>
-      <c r="S41">
-        <v>0</v>
-      </c>
-      <c r="T41">
-        <v>0</v>
-      </c>
-      <c r="U41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A42" s="5"/>
       <c r="B42" s="5" t="s">
         <v>17</v>
@@ -2477,35 +2002,17 @@
       <c r="K42">
         <v>17.12</v>
       </c>
+      <c r="L42">
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="M42">
-        <v>5.0000000000000001E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N42">
-        <v>0</v>
-      </c>
-      <c r="O42">
         <v>0.15440000000000001</v>
       </c>
-      <c r="P42" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q42" t="s">
-        <v>80</v>
-      </c>
-      <c r="R42" t="s">
-        <v>81</v>
-      </c>
-      <c r="S42">
-        <v>0</v>
-      </c>
-      <c r="T42">
-        <v>0</v>
-      </c>
-      <c r="U42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A43" s="5" t="s">
         <v>18</v>
       </c>
@@ -2534,35 +2041,17 @@
       <c r="K43">
         <v>25.83</v>
       </c>
+      <c r="L43">
+        <v>4.0000000000000002E-4</v>
+      </c>
       <c r="M43">
-        <v>4.0000000000000002E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N43">
-        <v>0</v>
-      </c>
-      <c r="O43">
         <v>0.22450000000000001</v>
       </c>
-      <c r="P43" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>80</v>
-      </c>
-      <c r="R43" t="s">
-        <v>81</v>
-      </c>
-      <c r="S43">
-        <v>0</v>
-      </c>
-      <c r="T43">
-        <v>0</v>
-      </c>
-      <c r="U43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A44" s="5"/>
       <c r="B44" s="5" t="s">
         <v>17</v>
@@ -2589,40 +2078,22 @@
       <c r="K44">
         <v>21.55</v>
       </c>
+      <c r="L44">
+        <v>1E-4</v>
+      </c>
       <c r="M44">
-        <v>1E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N44">
-        <v>0</v>
-      </c>
-      <c r="O44">
         <v>0.18890000000000001</v>
       </c>
-      <c r="P44" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>80</v>
-      </c>
-      <c r="R44" t="s">
-        <v>81</v>
-      </c>
-      <c r="S44">
-        <v>0</v>
-      </c>
-      <c r="T44">
-        <v>0</v>
-      </c>
-      <c r="U44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A47" s="5" t="s">
         <v>15</v>
       </c>
@@ -2651,35 +2122,17 @@
       <c r="K47">
         <v>14.21</v>
       </c>
+      <c r="L47">
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="M47">
-        <v>5.0000000000000001E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N47">
-        <v>0</v>
-      </c>
-      <c r="O47">
         <v>0.1009</v>
       </c>
-      <c r="P47" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>80</v>
-      </c>
-      <c r="R47" t="s">
-        <v>81</v>
-      </c>
-      <c r="S47">
-        <v>0</v>
-      </c>
-      <c r="T47">
-        <v>0</v>
-      </c>
-      <c r="U47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A48" s="5"/>
       <c r="B48" s="5" t="s">
         <v>17</v>
@@ -2706,35 +2159,17 @@
       <c r="K48">
         <v>21.21</v>
       </c>
+      <c r="L48">
+        <v>8.9999999999999998E-4</v>
+      </c>
       <c r="M48">
-        <v>8.9999999999999998E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N48">
-        <v>0</v>
-      </c>
-      <c r="O48">
         <v>0.20280000000000001</v>
       </c>
-      <c r="P48" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q48" t="s">
-        <v>80</v>
-      </c>
-      <c r="R48" t="s">
-        <v>81</v>
-      </c>
-      <c r="S48">
-        <v>0</v>
-      </c>
-      <c r="T48">
-        <v>0</v>
-      </c>
-      <c r="U48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A49" s="5" t="s">
         <v>18</v>
       </c>
@@ -2763,35 +2198,17 @@
       <c r="K49">
         <v>45.71</v>
       </c>
+      <c r="L49">
+        <v>2.0000000000000001E-4</v>
+      </c>
       <c r="M49">
-        <v>2.0000000000000001E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N49">
-        <v>0</v>
-      </c>
-      <c r="O49">
         <v>0.25659999999999999</v>
       </c>
-      <c r="P49" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>80</v>
-      </c>
-      <c r="R49" t="s">
-        <v>81</v>
-      </c>
-      <c r="S49">
-        <v>0</v>
-      </c>
-      <c r="T49">
-        <v>0</v>
-      </c>
-      <c r="U49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A50" s="5"/>
       <c r="B50" s="5" t="s">
         <v>17</v>
@@ -2818,43 +2235,25 @@
       <c r="K50">
         <v>31.23</v>
       </c>
+      <c r="L50">
+        <v>1E-4</v>
+      </c>
       <c r="M50">
-        <v>1E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N50">
-        <v>0</v>
-      </c>
-      <c r="O50">
         <v>0.31559999999999999</v>
       </c>
-      <c r="P50" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>80</v>
-      </c>
-      <c r="R50" t="s">
-        <v>81</v>
-      </c>
-      <c r="S50">
-        <v>0</v>
-      </c>
-      <c r="T50">
-        <v>0</v>
-      </c>
-      <c r="U50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A51" s="3"/>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A53" s="5" t="s">
         <v>15</v>
       </c>
@@ -2883,35 +2282,17 @@
       <c r="K53">
         <v>6.1</v>
       </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
       <c r="M53">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="N53">
-        <v>0</v>
-      </c>
-      <c r="O53">
         <v>6.8699999999999997E-2</v>
       </c>
-      <c r="P53" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>80</v>
-      </c>
-      <c r="R53" t="s">
-        <v>81</v>
-      </c>
-      <c r="S53">
-        <v>0</v>
-      </c>
-      <c r="T53">
-        <v>0</v>
-      </c>
-      <c r="U53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A54" s="5"/>
       <c r="B54" s="5" t="s">
         <v>17</v>
@@ -2938,35 +2319,17 @@
       <c r="K54">
         <v>4.34</v>
       </c>
+      <c r="L54">
+        <v>1E-4</v>
+      </c>
       <c r="M54">
-        <v>1E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N54">
-        <v>0</v>
-      </c>
-      <c r="O54">
         <v>7.1599999999999997E-2</v>
       </c>
-      <c r="P54" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q54" t="s">
-        <v>80</v>
-      </c>
-      <c r="R54" t="s">
-        <v>81</v>
-      </c>
-      <c r="S54">
-        <v>0</v>
-      </c>
-      <c r="T54">
-        <v>0</v>
-      </c>
-      <c r="U54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A55" s="5" t="s">
         <v>18</v>
       </c>
@@ -2995,35 +2358,17 @@
       <c r="K55">
         <v>4.26</v>
       </c>
+      <c r="L55">
+        <v>4.0000000000000002E-4</v>
+      </c>
       <c r="M55">
-        <v>4.0000000000000002E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N55">
-        <v>0</v>
-      </c>
-      <c r="O55">
         <v>5.33E-2</v>
       </c>
-      <c r="P55" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q55" t="s">
-        <v>80</v>
-      </c>
-      <c r="R55" t="s">
-        <v>81</v>
-      </c>
-      <c r="S55">
-        <v>0</v>
-      </c>
-      <c r="T55">
-        <v>0</v>
-      </c>
-      <c r="U55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="s">
         <v>17</v>
@@ -3050,40 +2395,22 @@
       <c r="K56">
         <v>7.48</v>
       </c>
+      <c r="L56">
+        <v>1E-4</v>
+      </c>
       <c r="M56">
-        <v>1E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N56">
-        <v>0</v>
-      </c>
-      <c r="O56">
         <v>7.9399999999999998E-2</v>
       </c>
-      <c r="P56" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>80</v>
-      </c>
-      <c r="R56" t="s">
-        <v>81</v>
-      </c>
-      <c r="S56">
-        <v>0</v>
-      </c>
-      <c r="T56">
-        <v>0</v>
-      </c>
-      <c r="U56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A59" s="5" t="s">
         <v>15</v>
       </c>
@@ -3112,35 +2439,17 @@
       <c r="K59">
         <v>19.260000000000002</v>
       </c>
+      <c r="L59">
+        <v>1.1999999999999999E-3</v>
+      </c>
       <c r="M59">
-        <v>1.1999999999999999E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N59">
-        <v>0</v>
-      </c>
-      <c r="O59">
         <v>0.10249999999999999</v>
       </c>
-      <c r="P59" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>80</v>
-      </c>
-      <c r="R59" t="s">
-        <v>81</v>
-      </c>
-      <c r="S59">
-        <v>0</v>
-      </c>
-      <c r="T59">
-        <v>0</v>
-      </c>
-      <c r="U59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A60" s="5"/>
       <c r="B60" s="5" t="s">
         <v>17</v>
@@ -3167,35 +2476,17 @@
       <c r="K60">
         <v>25.39</v>
       </c>
+      <c r="L60">
+        <v>2.9999999999999997E-4</v>
+      </c>
       <c r="M60">
-        <v>2.9999999999999997E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N60">
-        <v>0</v>
-      </c>
-      <c r="O60">
         <v>0.2261</v>
       </c>
-      <c r="P60" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q60" t="s">
-        <v>80</v>
-      </c>
-      <c r="R60" t="s">
-        <v>81</v>
-      </c>
-      <c r="S60">
-        <v>0</v>
-      </c>
-      <c r="T60">
-        <v>0</v>
-      </c>
-      <c r="U60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A61" s="5" t="s">
         <v>18</v>
       </c>
@@ -3224,35 +2515,17 @@
       <c r="K61">
         <v>54.89</v>
       </c>
+      <c r="L61">
+        <v>8.9999999999999998E-4</v>
+      </c>
       <c r="M61">
-        <v>8.9999999999999998E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N61">
-        <v>0</v>
-      </c>
-      <c r="O61">
         <v>0.38369999999999999</v>
       </c>
-      <c r="P61" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>80</v>
-      </c>
-      <c r="R61" t="s">
-        <v>81</v>
-      </c>
-      <c r="S61">
-        <v>0</v>
-      </c>
-      <c r="T61">
-        <v>0</v>
-      </c>
-      <c r="U61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
         <v>17</v>
@@ -3279,40 +2552,22 @@
       <c r="K62">
         <v>34.74</v>
       </c>
+      <c r="L62">
+        <v>4.0000000000000002E-4</v>
+      </c>
       <c r="M62">
-        <v>4.0000000000000002E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N62">
-        <v>0</v>
-      </c>
-      <c r="O62">
         <v>0.39269999999999999</v>
       </c>
-      <c r="P62" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q62" t="s">
-        <v>80</v>
-      </c>
-      <c r="R62" t="s">
-        <v>81</v>
-      </c>
-      <c r="S62">
-        <v>0</v>
-      </c>
-      <c r="T62">
-        <v>0</v>
-      </c>
-      <c r="U62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A65" s="5" t="s">
         <v>15</v>
       </c>
@@ -3341,35 +2596,17 @@
       <c r="K65">
         <v>14.79</v>
       </c>
+      <c r="L65">
+        <v>1.6999999999999999E-3</v>
+      </c>
       <c r="M65">
-        <v>1.6999999999999999E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N65">
-        <v>0</v>
-      </c>
-      <c r="O65">
         <v>8.8800000000000004E-2</v>
       </c>
-      <c r="P65" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>80</v>
-      </c>
-      <c r="R65" t="s">
-        <v>81</v>
-      </c>
-      <c r="S65">
-        <v>0</v>
-      </c>
-      <c r="T65">
-        <v>0</v>
-      </c>
-      <c r="U65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A66" s="5"/>
       <c r="B66" s="5" t="s">
         <v>17</v>
@@ -3396,35 +2633,17 @@
       <c r="K66">
         <v>23.09</v>
       </c>
+      <c r="L66">
+        <v>1.6999999999999999E-3</v>
+      </c>
       <c r="M66">
-        <v>1.6999999999999999E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N66">
-        <v>0</v>
-      </c>
-      <c r="O66">
         <v>0.16650000000000001</v>
       </c>
-      <c r="P66" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>80</v>
-      </c>
-      <c r="R66" t="s">
-        <v>81</v>
-      </c>
-      <c r="S66">
-        <v>0</v>
-      </c>
-      <c r="T66">
-        <v>0</v>
-      </c>
-      <c r="U66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A67" s="5" t="s">
         <v>18</v>
       </c>
@@ -3453,35 +2672,17 @@
       <c r="K67">
         <v>15.89</v>
       </c>
+      <c r="L67">
+        <v>5.0000000000000001E-4</v>
+      </c>
       <c r="M67">
-        <v>5.0000000000000001E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N67">
-        <v>0</v>
-      </c>
-      <c r="O67">
         <v>9.5100000000000004E-2</v>
       </c>
-      <c r="P67" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q67" t="s">
-        <v>80</v>
-      </c>
-      <c r="R67" t="s">
-        <v>81</v>
-      </c>
-      <c r="S67">
-        <v>0</v>
-      </c>
-      <c r="T67">
-        <v>0</v>
-      </c>
-      <c r="U67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A68" s="5"/>
       <c r="B68" s="5" t="s">
         <v>17</v>
@@ -3508,43 +2709,25 @@
       <c r="K68">
         <v>16.239999999999998</v>
       </c>
+      <c r="L68">
+        <v>1E-3</v>
+      </c>
       <c r="M68">
-        <v>1E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N68">
-        <v>0</v>
-      </c>
-      <c r="O68">
         <v>0.18210000000000001</v>
       </c>
-      <c r="P68" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q68" t="s">
-        <v>80</v>
-      </c>
-      <c r="R68" t="s">
-        <v>81</v>
-      </c>
-      <c r="S68">
-        <v>0</v>
-      </c>
-      <c r="T68">
-        <v>0</v>
-      </c>
-      <c r="U68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A71" s="5" t="s">
         <v>15</v>
       </c>
@@ -3573,35 +2756,17 @@
       <c r="K71">
         <v>11.08</v>
       </c>
+      <c r="L71">
+        <v>3.0999999999999999E-3</v>
+      </c>
       <c r="M71">
-        <v>3.0999999999999999E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N71">
-        <v>0</v>
-      </c>
-      <c r="O71">
         <v>7.5399999999999995E-2</v>
       </c>
-      <c r="P71" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>80</v>
-      </c>
-      <c r="R71" t="s">
-        <v>81</v>
-      </c>
-      <c r="S71">
-        <v>0</v>
-      </c>
-      <c r="T71">
-        <v>0</v>
-      </c>
-      <c r="U71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A72" s="5"/>
       <c r="B72" s="5" t="s">
         <v>17</v>
@@ -3628,35 +2793,17 @@
       <c r="K72">
         <v>14.77</v>
       </c>
+      <c r="L72">
+        <v>1E-4</v>
+      </c>
       <c r="M72">
-        <v>1E-4</v>
+        <v>0.3</v>
       </c>
       <c r="N72">
-        <v>0</v>
-      </c>
-      <c r="O72">
         <v>0.12609999999999999</v>
       </c>
-      <c r="P72" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q72" t="s">
-        <v>80</v>
-      </c>
-      <c r="R72" t="s">
-        <v>81</v>
-      </c>
-      <c r="S72">
-        <v>0</v>
-      </c>
-      <c r="T72">
-        <v>0</v>
-      </c>
-      <c r="U72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A73" s="5" t="s">
         <v>18</v>
       </c>
@@ -3685,35 +2832,17 @@
       <c r="K73">
         <v>30.78</v>
       </c>
+      <c r="L73">
+        <v>1.1000000000000001E-3</v>
+      </c>
       <c r="M73">
-        <v>1.1000000000000001E-3</v>
+        <v>0.3</v>
       </c>
       <c r="N73">
-        <v>0</v>
-      </c>
-      <c r="O73">
         <v>0.18</v>
       </c>
-      <c r="P73" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q73" t="s">
-        <v>80</v>
-      </c>
-      <c r="R73" t="s">
-        <v>81</v>
-      </c>
-      <c r="S73">
-        <v>0</v>
-      </c>
-      <c r="T73">
-        <v>0</v>
-      </c>
-      <c r="U73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A74" s="5"/>
       <c r="B74" s="5" t="s">
         <v>17</v>
@@ -3740,32 +2869,14 @@
       <c r="K74">
         <v>27.86</v>
       </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
       <c r="M74">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="N74">
-        <v>0</v>
-      </c>
-      <c r="O74">
         <v>0.21959999999999999</v>
-      </c>
-      <c r="P74" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>80</v>
-      </c>
-      <c r="R74" t="s">
-        <v>81</v>
-      </c>
-      <c r="S74">
-        <v>0</v>
-      </c>
-      <c r="T74">
-        <v>0</v>
-      </c>
-      <c r="U74">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>